<commit_message>
Réseau V1 (DMVPN, VLANs, RipV2)
</commit_message>
<xml_diff>
--- a/Prod/Infra/Réseau/Plan d'adressage/VLSM.xlsx
+++ b/Prod/Infra/Réseau/Plan d'adressage/VLSM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>@réseau</t>
   </si>
@@ -61,9 +61,6 @@
     <t>10.0.0.0</t>
   </si>
   <si>
-    <t>172.2.0.0</t>
-  </si>
-  <si>
     <t>10.1.255.255</t>
   </si>
   <si>
@@ -80,6 +77,27 @@
   </si>
   <si>
     <t>10.2.3.254</t>
+  </si>
+  <si>
+    <t>10.2.0.0</t>
+  </si>
+  <si>
+    <t>/25 = 255.255.255.128</t>
+  </si>
+  <si>
+    <t>10.2.4.0</t>
+  </si>
+  <si>
+    <t>10.2.4.1</t>
+  </si>
+  <si>
+    <t>10.2.4.126</t>
+  </si>
+  <si>
+    <t>10.2.4.127</t>
+  </si>
+  <si>
+    <t>Routeurs VPN</t>
   </si>
 </sst>
 </file>
@@ -479,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,13 +553,13 @@
         <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -558,16 +576,42 @@
         <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3">
+        <v>100</v>
+      </c>
+      <c r="C5" s="4">
+        <v>126</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>